<commit_message>
Epsilon Constrain Method for multi-objective optimization and Ensure Feasibility
</commit_message>
<xml_diff>
--- a/hypatia/examples/Planning_teaching/config.xlsx
+++ b/hypatia/examples/Planning_teaching/config.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="17" documentId="11_399507946124473CD69F2D2E2B28EDF8608B3BFE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB66216F-E043-48E2-9099-9E0A9B5C0682}"/>
   <bookViews>
-    <workbookView xWindow="-4680" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Techs" sheetId="1" r:id="rId1"/>
@@ -631,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1202,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1239,6 +1239,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100241E96938535DD4B921FCDFB54345D30" ma:contentTypeVersion="16" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="ea9f1ad5a580c8ec0c54747f8c275290">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e" xmlns:ns3="e67e9a88-35e1-4b39-8da9-a609eb308282" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a21d2b210d3c14c0eb20b1c12c2a17c" ns2:_="" ns3:_="">
     <xsd:import namespace="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e"/>
@@ -1481,19 +1490,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2AC6781-9D25-4D8C-9F2E-53294FC6CF02}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24802015-4ADE-4956-97E7-F806D57E32A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24802015-4ADE-4956-97E7-F806D57E32A9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2AC6781-9D25-4D8C-9F2E-53294FC6CF02}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e"/>
+    <ds:schemaRef ds:uri="e67e9a88-35e1-4b39-8da9-a609eb308282"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>